<commit_message>
Task 2 - identifies the column positions of credentials header
The system detect the "Account Number" and "PAN Number" headers in a dataset and determine their column positions.
and randomises the account number in single step
</commit_message>
<xml_diff>
--- a/Task 1 Kcs/input.xlsx
+++ b/Task 1 Kcs/input.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tasks KCS\Tasks-KCS\Task 1 Kcs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Task Kcs\Tasks-KCS-Task1\Task 1 Kcs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC8426BB-90CB-40BA-8A65-ADB663E68121}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A1AED09-2AA5-4153-BCB7-B8B75E15A7E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2196" yWindow="2196" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,12 +25,15 @@
     <t>Name</t>
   </si>
   <si>
+    <t>Account No</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
     <t>PAN Number</t>
   </si>
   <si>
-    <t>Subject</t>
-  </si>
-  <si>
     <t>Marks</t>
   </si>
   <si>
@@ -46,31 +49,28 @@
     <t>Umesh</t>
   </si>
   <si>
+    <t>Cyber Security</t>
+  </si>
+  <si>
+    <t>Mathematics</t>
+  </si>
+  <si>
+    <t>Computer Science</t>
+  </si>
+  <si>
+    <t>Software Engineering</t>
+  </si>
+  <si>
+    <t>ABCDE1111D</t>
+  </si>
+  <si>
     <t>ABCDE2222B</t>
   </si>
   <si>
-    <t>Cyber Security</t>
-  </si>
-  <si>
-    <t>Mathematics</t>
-  </si>
-  <si>
-    <t>Computer Science</t>
-  </si>
-  <si>
-    <t>Software Engineering</t>
-  </si>
-  <si>
-    <t>ABCDE1111D</t>
-  </si>
-  <si>
     <t>ABCDE3333C</t>
   </si>
   <si>
     <t>ABCDE4444A</t>
-  </si>
-  <si>
-    <t>Account No</t>
   </si>
 </sst>
 </file>
@@ -441,15 +441,10 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="24.6640625" customWidth="1"/>
-    <col min="3" max="3" width="19.88671875" customWidth="1"/>
-    <col min="4" max="4" width="18.109375" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
@@ -459,10 +454,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -470,274 +465,274 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>11111111</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2">
+        <v>76</v>
+      </c>
+      <c r="E2" t="s">
         <v>13</v>
-      </c>
-      <c r="C2">
-        <v>11111111</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2">
-        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>11111111</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3">
+        <v>99</v>
+      </c>
+      <c r="E3" t="s">
         <v>13</v>
-      </c>
-      <c r="C3">
-        <v>11111111</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3">
-        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>11111111</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4">
+        <v>84</v>
+      </c>
+      <c r="E4" t="s">
         <v>13</v>
-      </c>
-      <c r="C4">
-        <v>11111111</v>
-      </c>
-      <c r="D4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4">
-        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>11111111</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5">
+        <v>87</v>
+      </c>
+      <c r="E5" t="s">
         <v>13</v>
-      </c>
-      <c r="C5">
-        <v>11111111</v>
-      </c>
-      <c r="D5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5">
-        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6">
+        <v>6</v>
+      </c>
+      <c r="B6">
         <v>22222222</v>
       </c>
-      <c r="D6" t="s">
+      <c r="C6" t="s">
         <v>9</v>
       </c>
-      <c r="E6">
+      <c r="D6">
         <v>96</v>
+      </c>
+      <c r="E6" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7">
+        <v>6</v>
+      </c>
+      <c r="B7">
         <v>22222222</v>
       </c>
-      <c r="D7" t="s">
+      <c r="C7" t="s">
         <v>10</v>
       </c>
-      <c r="E7">
+      <c r="D7">
         <v>82</v>
+      </c>
+      <c r="E7" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8">
+        <v>6</v>
+      </c>
+      <c r="B8">
         <v>22222222</v>
       </c>
-      <c r="D8" t="s">
+      <c r="C8" t="s">
         <v>11</v>
       </c>
-      <c r="E8">
+      <c r="D8">
         <v>71</v>
+      </c>
+      <c r="E8" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9">
+        <v>6</v>
+      </c>
+      <c r="B9">
         <v>22222222</v>
       </c>
-      <c r="D9" t="s">
+      <c r="C9" t="s">
         <v>12</v>
       </c>
-      <c r="E9">
+      <c r="D9">
         <v>89</v>
+      </c>
+      <c r="E9" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10">
+        <v>7</v>
+      </c>
+      <c r="B10">
         <v>33333333</v>
       </c>
-      <c r="D10" t="s">
+      <c r="C10" t="s">
         <v>9</v>
       </c>
-      <c r="E10">
+      <c r="D10">
         <v>72</v>
+      </c>
+      <c r="E10" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11">
+        <v>7</v>
+      </c>
+      <c r="B11">
         <v>33333333</v>
       </c>
-      <c r="D11" t="s">
+      <c r="C11" t="s">
         <v>10</v>
       </c>
-      <c r="E11">
+      <c r="D11">
         <v>63</v>
+      </c>
+      <c r="E11" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12">
+        <v>7</v>
+      </c>
+      <c r="B12">
         <v>33333333</v>
       </c>
-      <c r="D12" t="s">
+      <c r="C12" t="s">
         <v>11</v>
       </c>
-      <c r="E12">
+      <c r="D12">
         <v>96</v>
+      </c>
+      <c r="E12" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13">
+        <v>7</v>
+      </c>
+      <c r="B13">
         <v>33333333</v>
       </c>
-      <c r="D13" t="s">
+      <c r="C13" t="s">
         <v>12</v>
       </c>
-      <c r="E13">
+      <c r="D13">
         <v>43</v>
+      </c>
+      <c r="E13" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14">
+        <v>8</v>
+      </c>
+      <c r="B14">
         <v>44444444</v>
       </c>
-      <c r="D14" t="s">
+      <c r="C14" t="s">
         <v>9</v>
       </c>
-      <c r="E14">
+      <c r="D14">
         <v>47</v>
+      </c>
+      <c r="E14" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15">
+        <v>8</v>
+      </c>
+      <c r="B15">
         <v>44444444</v>
       </c>
-      <c r="D15" t="s">
+      <c r="C15" t="s">
         <v>10</v>
       </c>
-      <c r="E15">
+      <c r="D15">
         <v>92</v>
+      </c>
+      <c r="E15" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16">
+        <v>8</v>
+      </c>
+      <c r="B16">
         <v>44444444</v>
       </c>
-      <c r="D16" t="s">
+      <c r="C16" t="s">
         <v>11</v>
       </c>
-      <c r="E16">
+      <c r="D16">
         <v>71</v>
+      </c>
+      <c r="E16" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>7</v>
-      </c>
-      <c r="B17" t="s">
-        <v>15</v>
-      </c>
-      <c r="C17">
+        <v>8</v>
+      </c>
+      <c r="B17">
         <v>44444444</v>
       </c>
-      <c r="D17" t="s">
+      <c r="C17" t="s">
         <v>12</v>
       </c>
-      <c r="E17">
+      <c r="D17">
         <v>65</v>
+      </c>
+      <c r="E17" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>